<commit_message>
Updated colors on the pin buffer mappings and copied buffer description table to datasheet
</commit_message>
<xml_diff>
--- a/pin_buffer_mappings.xlsx
+++ b/pin_buffer_mappings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dowster\Projects\bmw-obc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dowster\repos\bmw-obc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00F7DA10-88FE-48E0-9004-427F8583533B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18A9BED-4EED-4837-9E15-DE97557BDA78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" activeTab="1" xr2:uid="{C83741DB-6D2D-4F6E-BDC0-74E7E3ABD789}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C83741DB-6D2D-4F6E-BDC0-74E7E3ABD789}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,12 +536,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -549,6 +543,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -978,12 +978,12 @@
       <selection activeCell="A13" sqref="A13:I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>81</v>
@@ -1007,7 +1007,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>84</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>92</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>100</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>108</v>
       </c>
@@ -1111,8 +1111,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -1163,7 +1163,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>66</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>84</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>Byte 1,Bit 6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>84</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>Byte 1,Bit 5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>84</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>Byte 2,Bit 3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>84</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>Byte 2,Bit 2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>84</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>Byte 2,Bit 1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>84</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>Byte 1,Bit 7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>84</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>Byte 1,Bit 4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>92</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>Byte 1,Bit 2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>92</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>Byte 1,Bit 1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>92</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>Byte 2,Bit 7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>92</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>Byte 2,Bit 6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>92</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>Byte 2,Bit 5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>92</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>Byte 1,Bit 3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>92</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>Byte 1,Bit 0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>100</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>Byte 0,Bit 6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>100</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>Byte 0,Bit 5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>100</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>Byte 3,Bit 3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>100</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>Byte 3,Bit 2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>100</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>Byte 3,Bit 1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>100</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>Byte 0,Bit 7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>100</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>Byte 0,Bit 4</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>108</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>Byte 0,Bit 2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>108</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>Byte 0,Bit 1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>108</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>Byte 3,Bit 7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>108</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>Byte 3,Bit 6</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>108</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>Byte 3,Bit 5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>108</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>Byte 0,Bit 3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>Byte 0,Bit 0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>136</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>0</v>
       </c>
       <c r="C56" t="str">
-        <f t="shared" ref="C49:C85" si="3">_xlfn.CONCAT("Byte ",LEFT(INDEX($B$8:$Q$11,MATCH($A56,$A$8:$A$11),MATCH($B56,$B$7:$Q$7)),SEARCH(",",INDEX($B$8:$Q$11,MATCH($A56,$A$8:$A$11),MATCH($B56,$B$7:$Q$7)))-1))</f>
+        <f t="shared" ref="C56:C85" si="3">_xlfn.CONCAT("Byte ",LEFT(INDEX($B$8:$Q$11,MATCH($A56,$A$8:$A$11),MATCH($B56,$B$7:$Q$7)),SEARCH(",",INDEX($B$8:$Q$11,MATCH($A56,$A$8:$A$11),MATCH($B56,$B$7:$Q$7)))-1))</f>
         <v>Byte 5</v>
       </c>
       <c r="D56" t="str">
@@ -1955,7 +1955,7 @@
         <v>Byte 5,Bit 4</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>136</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>Byte 5,Bit 2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>136</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>Byte 5,Bit 0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>136</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>Byte 6,Bit 7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>136</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>Byte 6,Bit 3</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>136</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>Byte 6,Bit 5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>136</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>Byte 6,Bit 1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>136</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>Byte 5,Bit 6</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>136</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>Byte 5,Bit 7</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>136</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>Byte 7,Bit 0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>136</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>Byte 5,Bit 5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>136</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>Byte 5,Bit 3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>136</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>Byte 5,Bit 1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>136</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>Byte 6,Bit 6</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>136</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>Byte 6,Bit 4</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>136</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>Byte 6,Bit 2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>137</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>Byte 4,Bit 3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>137</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>Byte 4,Bit 1</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>137</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>Byte 11,Bit 7</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>137</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>Byte 7,Bit 7</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>137</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>Byte 7,Bit 3</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>137</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>Byte 7,Bit 5</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>137</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>Byte 7,Bit 1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>137</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>Byte 4,Bit 5</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>137</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>Byte 4,Bit 6</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>137</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>Byte 8,Bit 0</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>137</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>Byte 4,Bit 4</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>137</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>Byte 4,Bit 2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>137</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>Byte 4,Bit 0</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>137</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>Byte 7,Bit 6</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>137</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>Byte 7,Bit 4</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>137</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>Byte 7,Bit 2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>138</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>Byte 11,Bit 3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>138</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>Byte 11,Bit 1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>138</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>Byte 10,Bit 7</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>138</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>Byte 8,Bit 7</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>138</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>Byte 8,Bit 3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>138</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>Byte 8,Bit 5</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>138</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>Byte 8,Bit 1</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>138</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>Byte 11,Bit 5</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>138</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>Byte 11,Bit 6</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>138</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>Byte 9,Bit 0</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>138</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>Byte 11,Bit 4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>138</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>Byte 11,Bit 2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>138</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>Byte 11,Bit 0</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>138</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>Byte 8,Bit 6</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>138</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>Byte 8,Bit 4</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>138</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>Byte 8,Bit 2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>140</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>Byte 10,Bit 2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>140</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>Byte 10,Bit 2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>140</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>Byte 10,Bit 0</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>140</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>Byte 9,Bit 6</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>140</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>Byte 9,Bit 4</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>140</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>Byte 9,Bit 4</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>140</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>Byte 9,Bit 1</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>140</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>Byte 10,Bit 5</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>140</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>Byte 10,Bit 6</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>140</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>Byte 9,Bit 7</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>140</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>Byte 10,Bit 4</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>140</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>Byte 10,Bit 3</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>140</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>Byte 10,Bit 1</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>140</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>Byte 9,Bit 5</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>140</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>Byte 9,Bit 3</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>140</v>
       </c>
@@ -3227,18 +3227,16 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection sqref="A1:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>128</v>
       </c>
@@ -3264,7 +3262,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>116</v>
       </c>
@@ -3301,7 +3299,7 @@
         <v>DIGIT 4,G</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>117</v>
       </c>
@@ -3338,7 +3336,7 @@
         <v>DIGIT 2,G</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>118</v>
       </c>
@@ -3373,7 +3371,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>119</v>
       </c>
@@ -3408,7 +3406,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>120</v>
       </c>
@@ -3444,72 +3442,72 @@
         <v>DIGIT 6,J</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="12" t="str">
+      <c r="B7" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A7,",",B$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A7,",",B$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,G1</v>
       </c>
-      <c r="C7" s="12" t="str">
+      <c r="C7" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A7,",",C$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A7,",",C$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,F</v>
       </c>
-      <c r="D7" s="12" t="str">
+      <c r="D7" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A7,",",D$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A7,",",D$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,H</v>
       </c>
-      <c r="E7" s="12" t="str">
+      <c r="E7" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A7,",",E$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A7,",",E$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,A1</v>
       </c>
-      <c r="F7" s="12" t="str">
+      <c r="F7" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A7,",",F$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A7,",",F$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,I</v>
       </c>
-      <c r="G7" s="12" t="str">
+      <c r="G7" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A7,",",G$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A7,",",G$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,A2</v>
       </c>
-      <c r="H7" s="12" t="str">
+      <c r="H7" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A7,",",H$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A7,",",H$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,J</v>
       </c>
-      <c r="I7" s="12" t="str">
+      <c r="I7" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A7,",",I$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A7,",",I$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,B</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="12" t="str">
+      <c r="B8" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A8,",",B$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A8,",",B$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,C</v>
       </c>
-      <c r="C8" s="12" t="str">
+      <c r="C8" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A8,",",C$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A8,",",C$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,K</v>
       </c>
-      <c r="D8" s="12" t="str">
+      <c r="D8" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A8,",",D$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A8,",",D$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,D2</v>
       </c>
-      <c r="E8" s="12" t="str">
+      <c r="E8" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A8,",",E$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A8,",",E$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,L</v>
       </c>
-      <c r="F8" s="12" t="str">
+      <c r="F8" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A8,",",F$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A8,",",F$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,D1</v>
       </c>
-      <c r="G8" s="12" t="str">
+      <c r="G8" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A8,",",G$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A8,",",G$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,M</v>
       </c>
-      <c r="H8" s="12" t="str">
+      <c r="H8" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A8,",",H$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A8,",",H$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,E</v>
       </c>
@@ -3517,7 +3515,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>123</v>
       </c>
@@ -3549,40 +3547,40 @@
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A9,",",H$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A9,",",H$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 6,E</v>
       </c>
-      <c r="I9" s="12" t="str">
+      <c r="I9" s="14" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A9,",",I$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A9,",",I$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 5,G2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="13" t="str">
+      <c r="B10" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A10,",",B$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A10,",",B$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,C</v>
       </c>
-      <c r="C10" s="13" t="str">
+      <c r="C10" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A10,",",C$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A10,",",C$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,K</v>
       </c>
-      <c r="D10" s="13" t="str">
+      <c r="D10" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A10,",",D$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A10,",",D$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,D2</v>
       </c>
-      <c r="E10" s="13" t="str">
+      <c r="E10" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A10,",",E$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A10,",",E$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,L</v>
       </c>
-      <c r="F10" s="13" t="str">
+      <c r="F10" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A10,",",F$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A10,",",F$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,D1</v>
       </c>
-      <c r="G10" s="13" t="str">
+      <c r="G10" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A10,",",G$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A10,",",G$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,M</v>
       </c>
-      <c r="H10" s="13" t="str">
+      <c r="H10" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A10,",",H$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A10,",",H$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,E</v>
       </c>
@@ -3591,81 +3589,81 @@
         <v>DIGIT 6,G2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="14" t="str">
+      <c r="B11" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A11,",",B$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A11,",",B$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,G2</v>
       </c>
-      <c r="C11" s="14" t="str">
+      <c r="C11" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A11,",",C$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A11,",",C$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,C</v>
       </c>
-      <c r="D11" s="14" t="str">
+      <c r="D11" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A11,",",D$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A11,",",D$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,K</v>
       </c>
-      <c r="E11" s="14" t="str">
+      <c r="E11" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A11,",",E$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A11,",",E$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,D1</v>
       </c>
-      <c r="F11" s="14" t="str">
+      <c r="F11" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A11,",",F$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A11,",",F$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,L</v>
       </c>
-      <c r="G11" s="14" t="str">
+      <c r="G11" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A11,",",G$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A11,",",G$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,M</v>
       </c>
-      <c r="H11" s="14" t="str">
+      <c r="H11" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A11,",",H$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A11,",",H$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,E</v>
       </c>
-      <c r="I11" s="13" t="str">
+      <c r="I11" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A11,",",I$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A11,",",I$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,G2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="13" t="str">
+      <c r="B12" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A12,",",B$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A12,",",B$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,B</v>
       </c>
-      <c r="C12" s="14" t="str">
+      <c r="C12" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A12,",",C$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A12,",",C$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,G1</v>
       </c>
-      <c r="D12" s="14" t="str">
+      <c r="D12" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A12,",",D$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A12,",",D$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,F</v>
       </c>
-      <c r="E12" s="14" t="str">
+      <c r="E12" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A12,",",E$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A12,",",E$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,H</v>
       </c>
-      <c r="F12" s="14" t="str">
+      <c r="F12" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A12,",",F$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A12,",",F$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,I</v>
       </c>
-      <c r="G12" s="14" t="str">
+      <c r="G12" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A12,",",G$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A12,",",G$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,A1</v>
       </c>
-      <c r="H12" s="14" t="str">
+      <c r="H12" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A12,",",H$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A12,",",H$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,J</v>
       </c>
-      <c r="I12" s="14" t="str">
+      <c r="I12" s="13" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A12,",",I$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A12,",",I$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 8,B</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>127</v>
       </c>
@@ -3673,31 +3671,31 @@
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A13,",",B$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A13,",",B$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 6,B</v>
       </c>
-      <c r="C13" s="13" t="str">
+      <c r="C13" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A13,",",C$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A13,",",C$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,G1</v>
       </c>
-      <c r="D13" s="13" t="str">
+      <c r="D13" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A13,",",D$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A13,",",D$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,F</v>
       </c>
-      <c r="E13" s="13" t="str">
+      <c r="E13" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A13,",",E$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A13,",",E$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,H</v>
       </c>
-      <c r="F13" s="13" t="str">
+      <c r="F13" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A13,",",F$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A13,",",F$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,A1</v>
       </c>
-      <c r="G13" s="13" t="str">
+      <c r="G13" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A13,",",G$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A13,",",G$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,I</v>
       </c>
-      <c r="H13" s="13" t="str">
+      <c r="H13" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A13,",",H$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A13,",",H$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,A2</v>
       </c>
-      <c r="I13" s="13" t="str">
+      <c r="I13" s="12" t="str">
         <f>_xlfn.CONCAT(INDEX(Sheet1!$A$28:$A$119,MATCH(_xlfn.CONCAT($A13,",",I$1),Sheet1!$E$28:$E$119,0)),",",INDEX(Sheet1!$B$28:$B$119,MATCH(_xlfn.CONCAT($A13,",",I$1),Sheet1!$E$28:$E$119,0)))</f>
         <v>DIGIT 7,J</v>
       </c>

</xml_diff>